<commit_message>
update javadoc for CellConverter
</commit_message>
<xml_diff>
--- a/src/test/data/convert.xlsx
+++ b/src/test/data/convert.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="14805" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="14805" windowHeight="7995" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="数値型" sheetId="1" r:id="rId1"/>
@@ -15,13 +15,14 @@
     <sheet name="列挙型" sheetId="7" r:id="rId6"/>
     <sheet name="リンク型" sheetId="6" r:id="rId7"/>
     <sheet name="JSR310" sheetId="8" r:id="rId8"/>
+    <sheet name="独自" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="333">
   <si>
     <t>数値型のテスト</t>
     <rPh sb="0" eb="2">
@@ -2099,6 +2100,44 @@
       <t>イガイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>独自のConverterのテスト</t>
+    <rPh sb="0" eb="2">
+      <t>ドクジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>独自の書式1</t>
+    <rPh sb="0" eb="2">
+      <t>ドクジ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ショシキ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>TODOリスト
+- 部屋の片付け
+- 買い物</t>
+    <rPh sb="10" eb="12">
+      <t>ヘヤ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>カタヅ</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>モノ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>独自の書式2</t>
   </si>
 </sst>
 </file>
@@ -2241,7 +2280,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2321,6 +2360,15 @@
     <xf numFmtId="22" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="177" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2663,7 +2711,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
@@ -6495,7 +6543,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -6809,4 +6857,44 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="3" max="3" width="26.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" s="33" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="B4" s="60" t="s">
+        <v>330</v>
+      </c>
+      <c r="C4" s="59" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B5" s="60" t="s">
+        <v>332</v>
+      </c>
+      <c r="C5" s="58"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>